<commit_message>
commit báo cáo xong
commit báo cáo xong
</commit_message>
<xml_diff>
--- a/Bao cao/sodo.xlsx
+++ b/Bao cao/sodo.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,16 +146,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -165,7 +164,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1914525" y="2667000"/>
+          <a:off x="685800" y="2686050"/>
           <a:ext cx="1323975" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -223,16 +222,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -241,7 +240,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3657600" y="2667000"/>
+          <a:off x="2286000" y="2705100"/>
           <a:ext cx="1323975" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -299,16 +298,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -317,7 +316,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5381625" y="2667000"/>
+          <a:off x="3886200" y="2695575"/>
           <a:ext cx="1323975" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -375,16 +374,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -393,7 +392,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6000750" y="1533524"/>
+          <a:off x="6305550" y="1514474"/>
           <a:ext cx="1352550" cy="609601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -579,6 +578,16 @@
             <a:t>Chat box</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>(developers)</a:t>
+          </a:r>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -784,16 +793,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>138114</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>128589</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>547689</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -805,8 +814,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3109914" y="1571625"/>
-          <a:ext cx="561975" cy="1628775"/>
+          <a:off x="2486026" y="966787"/>
+          <a:ext cx="581025" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -831,16 +840,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>509589</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>547689</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>52389</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -851,9 +860,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="3981451" y="2328862"/>
-          <a:ext cx="561975" cy="114300"/>
+        <a:xfrm rot="5400000">
+          <a:off x="3276601" y="1776412"/>
+          <a:ext cx="600075" cy="1257300"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -881,13 +890,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>547688</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>557213</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>280988</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -899,8 +908,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4843463" y="1466849"/>
-          <a:ext cx="561975" cy="1838325"/>
+          <a:off x="4081463" y="2228850"/>
+          <a:ext cx="590550" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1160,16 +1169,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>547688</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1181,8 +1190,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="6922295" y="592931"/>
-          <a:ext cx="695324" cy="1185863"/>
+          <a:off x="7084220" y="735806"/>
+          <a:ext cx="676274" cy="881063"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1264,75 +1273,6 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t> sách bạn bè user</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600">
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Rectangle 33"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12506325" y="2638425"/>
-          <a:ext cx="1323975" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Danh </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>sách bạn bè page</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1600">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1392,29 +1332,105 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>566737</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="2714625"/>
+          <a:ext cx="1323975" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Chia sẻ</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Fanpage</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="38" name="Elbow Connector 37"/>
+        <xdr:cNvPr id="22" name="Elbow Connector 21"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="7" idx="2"/>
-          <a:endCxn id="34" idx="0"/>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="26" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="12096750" y="1566862"/>
-          <a:ext cx="514350" cy="1628775"/>
+          <a:off x="4867275" y="1443037"/>
+          <a:ext cx="609600" cy="1933575"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1705,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>